<commit_message>
All edits to Templates -04/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.1 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6398" uniqueCount="1983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6399" uniqueCount="1983">
   <si>
     <t>PS</t>
   </si>
@@ -5963,9 +5963,6 @@
     <t>NE</t>
   </si>
   <si>
-    <t>NE+SE?</t>
-  </si>
-  <si>
     <t>S[Sh]+N[s]</t>
   </si>
   <si>
@@ -5976,19 +5973,28 @@
   </si>
   <si>
     <t>Re?</t>
+  </si>
+  <si>
+    <t>PS-11.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -6178,200 +6184,203 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6656,10 +6665,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U2195" sqref="U2195"/>
+      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -53591,7 +53600,7 @@
       <c r="R1280" s="7"/>
       <c r="V1280" s="48"/>
     </row>
-    <row r="1281" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1281" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1281" s="21"/>
       <c r="F1281" s="21"/>
       <c r="G1281" s="21"/>
@@ -53623,7 +53632,7 @@
       <c r="R1281" s="7"/>
       <c r="V1281" s="48"/>
     </row>
-    <row r="1282" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1282" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1282" s="21"/>
       <c r="F1282" s="21"/>
       <c r="G1282" s="21"/>
@@ -53659,7 +53668,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="1283" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1283" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1283" s="21"/>
       <c r="F1283" s="21"/>
       <c r="G1283" s="21"/>
@@ -53697,7 +53706,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="1284" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1284" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1284" s="21"/>
       <c r="F1284" s="21"/>
       <c r="G1284" s="21"/>
@@ -53729,7 +53738,7 @@
       <c r="R1284" s="7"/>
       <c r="V1284" s="48"/>
     </row>
-    <row r="1285" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1285" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1285" s="21"/>
       <c r="F1285" s="21"/>
       <c r="G1285" s="21"/>
@@ -53761,7 +53770,7 @@
       <c r="R1285" s="7"/>
       <c r="V1285" s="48"/>
     </row>
-    <row r="1286" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1286" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1286" s="21"/>
       <c r="F1286" s="21"/>
       <c r="G1286" s="21"/>
@@ -53797,7 +53806,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="1287" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1287" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1287" s="21"/>
       <c r="F1287" s="21"/>
       <c r="G1287" s="21"/>
@@ -53829,7 +53838,7 @@
       <c r="R1287" s="7"/>
       <c r="V1287" s="48"/>
     </row>
-    <row r="1288" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1288" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1288" s="21"/>
       <c r="F1288" s="21"/>
       <c r="G1288" s="21"/>
@@ -53861,7 +53870,7 @@
       <c r="R1288" s="7"/>
       <c r="V1288" s="48"/>
     </row>
-    <row r="1289" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1289" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1289" s="21"/>
       <c r="F1289" s="21"/>
       <c r="G1289" s="21"/>
@@ -53897,7 +53906,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="1290" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1290" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1290" s="21"/>
       <c r="F1290" s="21"/>
       <c r="G1290" s="21"/>
@@ -53931,7 +53940,7 @@
       <c r="R1290" s="7"/>
       <c r="V1290" s="48"/>
     </row>
-    <row r="1291" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1291" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1291" s="21"/>
       <c r="F1291" s="21"/>
       <c r="G1291" s="21"/>
@@ -53965,7 +53974,10 @@
       <c r="R1291" s="7"/>
       <c r="V1291" s="48"/>
     </row>
-    <row r="1292" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1292" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="D1292" s="67" t="s">
+        <v>1982</v>
+      </c>
       <c r="E1292" s="21"/>
       <c r="F1292" s="21"/>
       <c r="G1292" s="21"/>
@@ -54000,13 +54012,13 @@
       <c r="Q1292" s="7"/>
       <c r="R1292" s="7"/>
       <c r="U1292" s="46" t="s">
-        <v>1978</v>
+        <v>1928</v>
       </c>
       <c r="V1292" s="48" t="s">
         <v>1777</v>
       </c>
     </row>
-    <row r="1293" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1293" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1293" s="21"/>
       <c r="F1293" s="21"/>
       <c r="G1293" s="21"/>
@@ -54038,7 +54050,7 @@
       <c r="R1293" s="7"/>
       <c r="V1293" s="48"/>
     </row>
-    <row r="1294" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1294" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1294" s="21"/>
       <c r="F1294" s="21"/>
       <c r="G1294" s="21"/>
@@ -54070,7 +54082,7 @@
       <c r="R1294" s="7"/>
       <c r="V1294" s="48"/>
     </row>
-    <row r="1295" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1295" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1295" s="21"/>
       <c r="F1295" s="21"/>
       <c r="G1295" s="21"/>
@@ -54106,7 +54118,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="1296" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1296" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1296" s="21"/>
       <c r="F1296" s="21"/>
       <c r="G1296" s="21"/>
@@ -62521,7 +62533,7 @@
         <v>1890</v>
       </c>
       <c r="T1538" s="7" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="V1538" s="48"/>
     </row>
@@ -68937,7 +68949,7 @@
         <v>1885</v>
       </c>
       <c r="T1776" s="7" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="V1776" s="48"/>
     </row>
@@ -76163,7 +76175,7 @@
         <v>1890</v>
       </c>
       <c r="T2049" s="7" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="V2049" s="48"/>
     </row>
@@ -79909,7 +79921,7 @@
         <v>1261</v>
       </c>
       <c r="U2195" s="7" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="V2195" s="48"/>
     </row>

</xml_diff>